<commit_message>
fixed variables and constraints, new constraint and ahc constraint missing
</commit_message>
<xml_diff>
--- a/irarc.xlsx
+++ b/irarc.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\prash\HiWi_2024\I-RARC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5032DC53-CBB1-407A-8C42-DEEBAD48D4DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{301C63A9-45B8-4814-91C2-F72CA7845DC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2340" yWindow="2610" windowWidth="21600" windowHeight="11265" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Nodes" sheetId="2" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2856" uniqueCount="1140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2856" uniqueCount="1171">
   <si>
     <t>Name</t>
   </si>
@@ -3293,9 +3293,6 @@
     <t>c64</t>
   </si>
   <si>
-    <t>Post-config connections per link</t>
-  </si>
-  <si>
     <t>c1</t>
   </si>
   <si>
@@ -3437,9 +3434,6 @@
     <t>c65</t>
   </si>
   <si>
-    <t>Pre-config connections per  link</t>
-  </si>
-  <si>
     <t>C_E</t>
   </si>
   <si>
@@ -3447,6 +3441,105 @@
   </si>
   <si>
     <t>C_All (CE + C_new)</t>
+  </si>
+  <si>
+    <t>nl1</t>
+  </si>
+  <si>
+    <t>nl2</t>
+  </si>
+  <si>
+    <t>nl3</t>
+  </si>
+  <si>
+    <t>Prnl-config connnlctions pnlr  link</t>
+  </si>
+  <si>
+    <t>Post-config connnlctions pnlr link</t>
+  </si>
+  <si>
+    <t>nl4</t>
+  </si>
+  <si>
+    <t>nl5</t>
+  </si>
+  <si>
+    <t>nl6</t>
+  </si>
+  <si>
+    <t>nl7</t>
+  </si>
+  <si>
+    <t>nl8</t>
+  </si>
+  <si>
+    <t>nl9</t>
+  </si>
+  <si>
+    <t>nl10</t>
+  </si>
+  <si>
+    <t>nl11</t>
+  </si>
+  <si>
+    <t>nl12</t>
+  </si>
+  <si>
+    <t>nl13</t>
+  </si>
+  <si>
+    <t>nl14</t>
+  </si>
+  <si>
+    <t>nl15</t>
+  </si>
+  <si>
+    <t>nl16</t>
+  </si>
+  <si>
+    <t>nl17</t>
+  </si>
+  <si>
+    <t>nl18</t>
+  </si>
+  <si>
+    <t>nl19</t>
+  </si>
+  <si>
+    <t>nl20</t>
+  </si>
+  <si>
+    <t>nl21</t>
+  </si>
+  <si>
+    <t>nl22</t>
+  </si>
+  <si>
+    <t>nl23</t>
+  </si>
+  <si>
+    <t>nl24</t>
+  </si>
+  <si>
+    <t>nl25</t>
+  </si>
+  <si>
+    <t>nl26</t>
+  </si>
+  <si>
+    <t>nl27</t>
+  </si>
+  <si>
+    <t>nl28</t>
+  </si>
+  <si>
+    <t>nl29</t>
+  </si>
+  <si>
+    <t>nl30</t>
+  </si>
+  <si>
+    <t>nl31</t>
   </si>
 </sst>
 </file>
@@ -3949,7 +4042,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:F32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F16" sqref="F16"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -3967,15 +4062,15 @@
         <v>37</v>
       </c>
       <c r="C1" t="s">
-        <v>1136</v>
+        <v>1141</v>
       </c>
       <c r="D1" t="s">
-        <v>1088</v>
+        <v>1142</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>47</v>
+        <v>1138</v>
       </c>
       <c r="B2" t="s">
         <v>899</v>
@@ -3986,7 +4081,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>49</v>
+        <v>1139</v>
       </c>
       <c r="B3" t="s">
         <v>900</v>
@@ -4000,7 +4095,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>51</v>
+        <v>1140</v>
       </c>
       <c r="B4" t="s">
         <v>901</v>
@@ -4014,7 +4109,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>52</v>
+        <v>1143</v>
       </c>
       <c r="B5" t="s">
         <v>903</v>
@@ -4028,7 +4123,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>53</v>
+        <v>1144</v>
       </c>
       <c r="B6" t="s">
         <v>908</v>
@@ -4042,7 +4137,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>54</v>
+        <v>1145</v>
       </c>
       <c r="B7" t="s">
         <v>909</v>
@@ -4056,7 +4151,7 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>56</v>
+        <v>1146</v>
       </c>
       <c r="B8" t="s">
         <v>910</v>
@@ -4067,7 +4162,7 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>58</v>
+        <v>1147</v>
       </c>
       <c r="B9" t="s">
         <v>911</v>
@@ -4081,7 +4176,7 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>60</v>
+        <v>1148</v>
       </c>
       <c r="B10" t="s">
         <v>912</v>
@@ -4095,7 +4190,7 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>62</v>
+        <v>1149</v>
       </c>
       <c r="B11" t="s">
         <v>913</v>
@@ -4109,7 +4204,7 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>64</v>
+        <v>1150</v>
       </c>
       <c r="B12" t="s">
         <v>914</v>
@@ -4120,7 +4215,7 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>66</v>
+        <v>1151</v>
       </c>
       <c r="B13" t="s">
         <v>918</v>
@@ -4134,7 +4229,7 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>68</v>
+        <v>1152</v>
       </c>
       <c r="B14" t="s">
         <v>920</v>
@@ -4148,7 +4243,7 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>69</v>
+        <v>1153</v>
       </c>
       <c r="B15" t="s">
         <v>927</v>
@@ -4159,7 +4254,7 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>71</v>
+        <v>1154</v>
       </c>
       <c r="B16" t="s">
         <v>928</v>
@@ -4173,7 +4268,7 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>72</v>
+        <v>1155</v>
       </c>
       <c r="B17" t="s">
         <v>929</v>
@@ -4187,7 +4282,7 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>73</v>
+        <v>1156</v>
       </c>
       <c r="B18" t="s">
         <v>930</v>
@@ -4201,7 +4296,7 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>75</v>
+        <v>1157</v>
       </c>
       <c r="B19" t="s">
         <v>931</v>
@@ -4215,7 +4310,7 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>77</v>
+        <v>1158</v>
       </c>
       <c r="B20" t="s">
         <v>932</v>
@@ -4229,7 +4324,7 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>79</v>
+        <v>1159</v>
       </c>
       <c r="B21" t="s">
         <v>933</v>
@@ -4243,7 +4338,7 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>81</v>
+        <v>1160</v>
       </c>
       <c r="B22" t="s">
         <v>934</v>
@@ -4257,7 +4352,7 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>83</v>
+        <v>1161</v>
       </c>
       <c r="B23" t="s">
         <v>935</v>
@@ -4271,7 +4366,7 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>84</v>
+        <v>1162</v>
       </c>
       <c r="B24" t="s">
         <v>937</v>
@@ -4285,7 +4380,7 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>86</v>
+        <v>1163</v>
       </c>
       <c r="B25" t="s">
         <v>942</v>
@@ -4299,7 +4394,7 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>88</v>
+        <v>1164</v>
       </c>
       <c r="B26" t="s">
         <v>943</v>
@@ -4313,7 +4408,7 @@
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>90</v>
+        <v>1165</v>
       </c>
       <c r="B27" t="s">
         <v>953</v>
@@ -4327,7 +4422,7 @@
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>92</v>
+        <v>1166</v>
       </c>
       <c r="B28" t="s">
         <v>954</v>
@@ -4341,7 +4436,7 @@
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>93</v>
+        <v>1167</v>
       </c>
       <c r="B29" t="s">
         <v>955</v>
@@ -4355,7 +4450,7 @@
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>95</v>
+        <v>1168</v>
       </c>
       <c r="B30" t="s">
         <v>956</v>
@@ -4369,7 +4464,7 @@
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>97</v>
+        <v>1169</v>
       </c>
       <c r="B31" t="s">
         <v>958</v>
@@ -4380,7 +4475,7 @@
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>99</v>
+        <v>1170</v>
       </c>
       <c r="B32" t="s">
         <v>960</v>
@@ -4415,16 +4510,16 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>1135</v>
+      </c>
+      <c r="B1" t="s">
         <v>1137</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1139</v>
       </c>
       <c r="C1" t="s">
         <v>37</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>1138</v>
+        <v>1136</v>
       </c>
       <c r="E1" t="s">
         <v>101</v>
@@ -4432,10 +4527,10 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>1089</v>
+        <v>1088</v>
       </c>
       <c r="B2" t="s">
-        <v>1089</v>
+        <v>1088</v>
       </c>
       <c r="C2" t="s">
         <v>103</v>
@@ -4449,10 +4544,10 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>1090</v>
+        <v>1089</v>
       </c>
       <c r="B3" t="s">
-        <v>1090</v>
+        <v>1089</v>
       </c>
       <c r="C3" t="s">
         <v>106</v>
@@ -4466,10 +4561,10 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>1091</v>
+        <v>1090</v>
       </c>
       <c r="B4" t="s">
-        <v>1091</v>
+        <v>1090</v>
       </c>
       <c r="C4" t="s">
         <v>109</v>
@@ -4517,10 +4612,10 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>1092</v>
+        <v>1091</v>
       </c>
       <c r="B7" t="s">
-        <v>1092</v>
+        <v>1091</v>
       </c>
       <c r="C7" t="s">
         <v>118</v>
@@ -4568,10 +4663,10 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>1093</v>
+        <v>1092</v>
       </c>
       <c r="B10" t="s">
-        <v>1093</v>
+        <v>1092</v>
       </c>
       <c r="C10" t="s">
         <v>127</v>
@@ -4585,10 +4680,10 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>1094</v>
+        <v>1093</v>
       </c>
       <c r="B11" t="s">
-        <v>1094</v>
+        <v>1093</v>
       </c>
       <c r="C11" t="s">
         <v>130</v>
@@ -4602,10 +4697,10 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>1095</v>
+        <v>1094</v>
       </c>
       <c r="B12" t="s">
-        <v>1095</v>
+        <v>1094</v>
       </c>
       <c r="C12" t="s">
         <v>133</v>
@@ -4619,10 +4714,10 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>1096</v>
+        <v>1095</v>
       </c>
       <c r="B13" t="s">
-        <v>1096</v>
+        <v>1095</v>
       </c>
       <c r="C13" t="s">
         <v>136</v>
@@ -4636,10 +4731,10 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>1097</v>
+        <v>1096</v>
       </c>
       <c r="B14" t="s">
-        <v>1097</v>
+        <v>1096</v>
       </c>
       <c r="C14" t="s">
         <v>139</v>
@@ -4653,10 +4748,10 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>1098</v>
+        <v>1097</v>
       </c>
       <c r="B15" t="s">
-        <v>1098</v>
+        <v>1097</v>
       </c>
       <c r="C15" t="s">
         <v>142</v>
@@ -4670,10 +4765,10 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>1099</v>
+        <v>1098</v>
       </c>
       <c r="B16" t="s">
-        <v>1099</v>
+        <v>1098</v>
       </c>
       <c r="C16" t="s">
         <v>145</v>
@@ -4687,10 +4782,10 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>1100</v>
+        <v>1099</v>
       </c>
       <c r="B17" t="s">
-        <v>1100</v>
+        <v>1099</v>
       </c>
       <c r="C17" t="s">
         <v>148</v>
@@ -4704,10 +4799,10 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>1101</v>
+        <v>1100</v>
       </c>
       <c r="B18" t="s">
-        <v>1101</v>
+        <v>1100</v>
       </c>
       <c r="C18" t="s">
         <v>151</v>
@@ -4721,10 +4816,10 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>1102</v>
+        <v>1101</v>
       </c>
       <c r="B19" t="s">
-        <v>1102</v>
+        <v>1101</v>
       </c>
       <c r="C19" t="s">
         <v>154</v>
@@ -4738,10 +4833,10 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>1103</v>
+        <v>1102</v>
       </c>
       <c r="B20" t="s">
-        <v>1103</v>
+        <v>1102</v>
       </c>
       <c r="C20" t="s">
         <v>157</v>
@@ -4755,10 +4850,10 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>1104</v>
+        <v>1103</v>
       </c>
       <c r="B21" t="s">
-        <v>1104</v>
+        <v>1103</v>
       </c>
       <c r="C21" t="s">
         <v>160</v>
@@ -4772,10 +4867,10 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>1105</v>
+        <v>1104</v>
       </c>
       <c r="B22" t="s">
-        <v>1105</v>
+        <v>1104</v>
       </c>
       <c r="C22" t="s">
         <v>163</v>
@@ -4789,10 +4884,10 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>1106</v>
+        <v>1105</v>
       </c>
       <c r="B23" t="s">
-        <v>1106</v>
+        <v>1105</v>
       </c>
       <c r="C23" t="s">
         <v>166</v>
@@ -4806,10 +4901,10 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>1107</v>
+        <v>1106</v>
       </c>
       <c r="B24" t="s">
-        <v>1107</v>
+        <v>1106</v>
       </c>
       <c r="C24" t="s">
         <v>169</v>
@@ -4840,10 +4935,10 @@
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>1108</v>
+        <v>1107</v>
       </c>
       <c r="B26" t="s">
-        <v>1108</v>
+        <v>1107</v>
       </c>
       <c r="C26" t="s">
         <v>175</v>
@@ -4857,10 +4952,10 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>1109</v>
+        <v>1108</v>
       </c>
       <c r="B27" t="s">
-        <v>1109</v>
+        <v>1108</v>
       </c>
       <c r="C27" t="s">
         <v>178</v>
@@ -4874,10 +4969,10 @@
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>1110</v>
+        <v>1109</v>
       </c>
       <c r="B28" t="s">
-        <v>1110</v>
+        <v>1109</v>
       </c>
       <c r="C28" t="s">
         <v>181</v>
@@ -4891,10 +4986,10 @@
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>1111</v>
+        <v>1110</v>
       </c>
       <c r="B29" t="s">
-        <v>1111</v>
+        <v>1110</v>
       </c>
       <c r="C29" t="s">
         <v>184</v>
@@ -4908,10 +5003,10 @@
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>1112</v>
+        <v>1111</v>
       </c>
       <c r="B30" t="s">
-        <v>1112</v>
+        <v>1111</v>
       </c>
       <c r="C30" t="s">
         <v>187</v>
@@ -4925,10 +5020,10 @@
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>1113</v>
+        <v>1112</v>
       </c>
       <c r="B31" t="s">
-        <v>1113</v>
+        <v>1112</v>
       </c>
       <c r="C31" t="s">
         <v>190</v>
@@ -4942,10 +5037,10 @@
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>1114</v>
+        <v>1113</v>
       </c>
       <c r="B32" t="s">
-        <v>1114</v>
+        <v>1113</v>
       </c>
       <c r="C32" t="s">
         <v>193</v>
@@ -4959,10 +5054,10 @@
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>1115</v>
+        <v>1114</v>
       </c>
       <c r="B33" t="s">
-        <v>1115</v>
+        <v>1114</v>
       </c>
       <c r="C33" t="s">
         <v>196</v>
@@ -4976,10 +5071,10 @@
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>1116</v>
+        <v>1115</v>
       </c>
       <c r="B34" t="s">
-        <v>1116</v>
+        <v>1115</v>
       </c>
       <c r="C34" t="s">
         <v>199</v>
@@ -5010,10 +5105,10 @@
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>1117</v>
+        <v>1116</v>
       </c>
       <c r="B36" t="s">
-        <v>1117</v>
+        <v>1116</v>
       </c>
       <c r="C36" t="s">
         <v>205</v>
@@ -5027,10 +5122,10 @@
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>1118</v>
+        <v>1117</v>
       </c>
       <c r="B37" t="s">
-        <v>1118</v>
+        <v>1117</v>
       </c>
       <c r="C37" t="s">
         <v>208</v>
@@ -5044,10 +5139,10 @@
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>1119</v>
+        <v>1118</v>
       </c>
       <c r="B38" t="s">
-        <v>1119</v>
+        <v>1118</v>
       </c>
       <c r="C38" t="s">
         <v>211</v>
@@ -5061,10 +5156,10 @@
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>1120</v>
+        <v>1119</v>
       </c>
       <c r="B39" t="s">
-        <v>1120</v>
+        <v>1119</v>
       </c>
       <c r="C39" t="s">
         <v>214</v>
@@ -5095,10 +5190,10 @@
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>1121</v>
+        <v>1120</v>
       </c>
       <c r="B41" t="s">
-        <v>1121</v>
+        <v>1120</v>
       </c>
       <c r="C41" t="s">
         <v>220</v>
@@ -5129,10 +5224,10 @@
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>1122</v>
+        <v>1121</v>
       </c>
       <c r="B43" t="s">
-        <v>1122</v>
+        <v>1121</v>
       </c>
       <c r="C43" t="s">
         <v>226</v>
@@ -5146,10 +5241,10 @@
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>1123</v>
+        <v>1122</v>
       </c>
       <c r="B44" t="s">
-        <v>1123</v>
+        <v>1122</v>
       </c>
       <c r="C44" t="s">
         <v>229</v>
@@ -5180,10 +5275,10 @@
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>1124</v>
+        <v>1123</v>
       </c>
       <c r="B46" t="s">
-        <v>1124</v>
+        <v>1123</v>
       </c>
       <c r="C46" t="s">
         <v>235</v>
@@ -5231,10 +5326,10 @@
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>1125</v>
+        <v>1124</v>
       </c>
       <c r="B49" t="s">
-        <v>1125</v>
+        <v>1124</v>
       </c>
       <c r="C49" t="s">
         <v>244</v>
@@ -5248,10 +5343,10 @@
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>1126</v>
+        <v>1125</v>
       </c>
       <c r="B50" t="s">
-        <v>1126</v>
+        <v>1125</v>
       </c>
       <c r="C50" t="s">
         <v>247</v>
@@ -5265,10 +5360,10 @@
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>1127</v>
+        <v>1126</v>
       </c>
       <c r="B51" t="s">
-        <v>1127</v>
+        <v>1126</v>
       </c>
       <c r="C51" t="s">
         <v>250</v>
@@ -5282,10 +5377,10 @@
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>1128</v>
+        <v>1127</v>
       </c>
       <c r="B52" t="s">
-        <v>1128</v>
+        <v>1127</v>
       </c>
       <c r="C52" t="s">
         <v>253</v>
@@ -5299,10 +5394,10 @@
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>1129</v>
+        <v>1128</v>
       </c>
       <c r="B53" t="s">
-        <v>1129</v>
+        <v>1128</v>
       </c>
       <c r="C53" t="s">
         <v>256</v>
@@ -5316,10 +5411,10 @@
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>1130</v>
+        <v>1129</v>
       </c>
       <c r="B54" t="s">
-        <v>1130</v>
+        <v>1129</v>
       </c>
       <c r="C54" t="s">
         <v>259</v>
@@ -5333,10 +5428,10 @@
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>1131</v>
+        <v>1130</v>
       </c>
       <c r="B55" t="s">
-        <v>1131</v>
+        <v>1130</v>
       </c>
       <c r="C55" t="s">
         <v>262</v>
@@ -5449,7 +5544,7 @@
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B62" t="s">
-        <v>1132</v>
+        <v>1131</v>
       </c>
       <c r="C62" t="s">
         <v>283</v>
@@ -5463,7 +5558,7 @@
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B63" t="s">
-        <v>1133</v>
+        <v>1132</v>
       </c>
       <c r="C63" t="s">
         <v>286</v>
@@ -5477,7 +5572,7 @@
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B64" t="s">
-        <v>1134</v>
+        <v>1133</v>
       </c>
       <c r="C64" t="s">
         <v>289</v>
@@ -5505,7 +5600,7 @@
     </row>
     <row r="66" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B66" t="s">
-        <v>1135</v>
+        <v>1134</v>
       </c>
       <c r="C66" t="s">
         <v>295</v>

</xml_diff>

<commit_message>
indices in constraints need to be fixed
</commit_message>
<xml_diff>
--- a/irarc.xlsx
+++ b/irarc.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\prash\HiWi_2024\I-RARC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{301C63A9-45B8-4814-91C2-F72CA7845DC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{838666FD-658F-4262-B809-074D343E9957}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2340" yWindow="2610" windowWidth="21600" windowHeight="11265" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7305" yWindow="4320" windowWidth="21600" windowHeight="11265" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Nodes" sheetId="2" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2856" uniqueCount="1171">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2857" uniqueCount="1132">
   <si>
     <t>Name</t>
   </si>
@@ -2918,135 +2918,9 @@
     <t>S-&gt;F-&gt;UL</t>
   </si>
   <si>
-    <t>Post-config demands per link</t>
-  </si>
-  <si>
-    <t>Pre-config demands per link</t>
-  </si>
-  <si>
-    <t>d2,d23,d39,d41,d42,d43,d45</t>
-  </si>
-  <si>
-    <t>d1,d4,d6,d7,d8,d23,d26,d39,d47</t>
-  </si>
-  <si>
-    <t>d3,d5,d9,d10,d11,d26,d41,d42,d43,d45,d47</t>
-  </si>
-  <si>
-    <t>d1,d14,d15,d16,d21,d24,d33</t>
-  </si>
-  <si>
-    <t>d17,d18,d32,d51</t>
-  </si>
-  <si>
-    <t>d6,d24,d32,d51</t>
-  </si>
-  <si>
-    <t>d6,d12,d13,d19,d20,d33,d55</t>
-  </si>
-  <si>
-    <t>d12,d16,d21,d27,d28,d33,d49,d50</t>
-  </si>
-  <si>
-    <t>d1,d2,d14,d15,d22,d23,d25,d26,d29,d30,d49,d50</t>
-  </si>
-  <si>
-    <t>d8,d22,d25,d31,d34,d40,d46</t>
-  </si>
-  <si>
-    <t>d12,d13,d16,d19,d20,d25,d40,d46,d52,d53,d54</t>
-  </si>
-  <si>
-    <t>d9,d11,d17,d38,d58</t>
-  </si>
-  <si>
-    <t>d3,d9,d19,d37,d49,d52,d58</t>
-  </si>
-  <si>
-    <t>d18,d20,d27,d28,d35,d36,d50,d53,d54</t>
-  </si>
-  <si>
-    <t>d11,d21,d51</t>
-  </si>
-  <si>
-    <t>d2,d4,d14,d31,d40</t>
-  </si>
-  <si>
-    <t>d5,d7,d29,d30,d34,d48,d56</t>
-  </si>
-  <si>
-    <t>d42,d59</t>
-  </si>
-  <si>
-    <t>d3,d10,d43,d44,d52,d55</t>
-  </si>
-  <si>
-    <t>d29,d48,d57</t>
-  </si>
-  <si>
-    <t>d30,d38,d45,d56</t>
-  </si>
-  <si>
-    <t>d18,d27,d35,d48,d53,d57,d59</t>
-  </si>
-  <si>
-    <t>d10,d28,d36,d37,d44,d54,d55</t>
-  </si>
-  <si>
-    <t>d11,d21,d30,d38,d45,d51,d56,d63,d65,d66</t>
-  </si>
-  <si>
-    <t>d10,d20,d29,d37,d44,d50,d55,d66</t>
-  </si>
-  <si>
-    <t>d9,d19,d28,d36,d43,d49,d54,d61,d65</t>
-  </si>
-  <si>
-    <t>d8,d35,d61,d63</t>
-  </si>
-  <si>
-    <t>d6,d33,d54,d55,d56</t>
-  </si>
-  <si>
-    <t>d32,d49,d50,d51</t>
-  </si>
-  <si>
-    <t>d31,d43,d44,d45</t>
-  </si>
-  <si>
-    <t>d2,d22,d28,d29,d30</t>
-  </si>
-  <si>
-    <t>d18,d27,d42,d48,d53</t>
-  </si>
-  <si>
-    <t>d17,d26,d52</t>
-  </si>
-  <si>
-    <t>d16,d25,d40,d52,d53</t>
-  </si>
-  <si>
-    <t>d15,d48</t>
-  </si>
-  <si>
-    <t>d14,d23,d40,d42</t>
-  </si>
-  <si>
-    <t>d1,d13,d19,d20,d21</t>
-  </si>
-  <si>
-    <t>d23,d25,d26,d27,d12</t>
-  </si>
-  <si>
-    <t>d1,d2,d3,d6,d8,d9,d10,d11</t>
-  </si>
-  <si>
     <t>no. of slots</t>
   </si>
   <si>
-    <t>Pre-config traffic per link</t>
-  </si>
-  <si>
     <t>total slots pre-config</t>
   </si>
   <si>
@@ -3452,12 +3326,6 @@
     <t>nl3</t>
   </si>
   <si>
-    <t>Prnl-config connnlctions pnlr  link</t>
-  </si>
-  <si>
-    <t>Post-config connnlctions pnlr link</t>
-  </si>
-  <si>
     <t>nl4</t>
   </si>
   <si>
@@ -3540,6 +3408,21 @@
   </si>
   <si>
     <t>nl31</t>
+  </si>
+  <si>
+    <t>Pre-config connelctions per  link</t>
+  </si>
+  <si>
+    <t>Post-config connections per link</t>
+  </si>
+  <si>
+    <t>slots per link</t>
+  </si>
+  <si>
+    <t>Pre-config connections per link</t>
+  </si>
+  <si>
+    <t>Pre-config traffic per link (1.25Gb)</t>
   </si>
 </sst>
 </file>
@@ -4042,8 +3925,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:F32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="D37" sqref="D37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4051,440 +3934,537 @@
     <col min="2" max="2" width="27.5703125" customWidth="1"/>
     <col min="3" max="3" width="44.28515625" customWidth="1"/>
     <col min="4" max="4" width="43.5703125" customWidth="1"/>
+    <col min="5" max="5" width="12.140625" customWidth="1"/>
     <col min="6" max="6" width="21.140625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>1030</v>
+        <v>988</v>
       </c>
       <c r="B1" t="s">
         <v>37</v>
       </c>
       <c r="C1" t="s">
-        <v>1141</v>
+        <v>1127</v>
       </c>
       <c r="D1" t="s">
-        <v>1142</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+        <v>1128</v>
+      </c>
+      <c r="E1" t="s">
+        <v>1129</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>1138</v>
+        <v>1096</v>
       </c>
       <c r="B2" t="s">
         <v>899</v>
       </c>
       <c r="D2" t="s">
-        <v>1058</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+        <v>1016</v>
+      </c>
+      <c r="E2">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>1139</v>
+        <v>1097</v>
       </c>
       <c r="B3" t="s">
         <v>900</v>
       </c>
       <c r="C3" t="s">
-        <v>1031</v>
+        <v>989</v>
       </c>
       <c r="D3" t="s">
-        <v>1059</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+        <v>1017</v>
+      </c>
+      <c r="E3">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>1140</v>
+        <v>1098</v>
       </c>
       <c r="B4" t="s">
         <v>901</v>
       </c>
       <c r="C4" t="s">
-        <v>1032</v>
+        <v>990</v>
       </c>
       <c r="D4" t="s">
-        <v>1060</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+        <v>1018</v>
+      </c>
+      <c r="E4">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>1143</v>
+        <v>1099</v>
       </c>
       <c r="B5" t="s">
         <v>903</v>
       </c>
       <c r="C5" t="s">
-        <v>1033</v>
+        <v>991</v>
       </c>
       <c r="D5" t="s">
-        <v>1061</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+        <v>1019</v>
+      </c>
+      <c r="E5">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>1144</v>
+        <v>1100</v>
       </c>
       <c r="B6" t="s">
         <v>908</v>
       </c>
       <c r="C6" t="s">
-        <v>1034</v>
+        <v>992</v>
       </c>
       <c r="D6" t="s">
-        <v>1062</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+        <v>1020</v>
+      </c>
+      <c r="E6">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>1145</v>
+        <v>1101</v>
       </c>
       <c r="B7" t="s">
         <v>909</v>
       </c>
       <c r="C7" t="s">
-        <v>1035</v>
+        <v>993</v>
       </c>
       <c r="D7" t="s">
-        <v>1063</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+        <v>1021</v>
+      </c>
+      <c r="E7">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>1146</v>
+        <v>1102</v>
       </c>
       <c r="B8" t="s">
         <v>910</v>
       </c>
       <c r="D8" t="s">
-        <v>1064</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+        <v>1022</v>
+      </c>
+      <c r="E8">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>1147</v>
+        <v>1103</v>
       </c>
       <c r="B9" t="s">
         <v>911</v>
       </c>
       <c r="C9" t="s">
-        <v>1036</v>
+        <v>994</v>
       </c>
       <c r="D9" t="s">
-        <v>1065</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+        <v>1023</v>
+      </c>
+      <c r="E9">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>1148</v>
+        <v>1104</v>
       </c>
       <c r="B10" t="s">
         <v>912</v>
       </c>
       <c r="C10" t="s">
-        <v>1037</v>
+        <v>995</v>
       </c>
       <c r="D10" t="s">
-        <v>1066</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+        <v>1024</v>
+      </c>
+      <c r="E10">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>1149</v>
+        <v>1105</v>
       </c>
       <c r="B11" t="s">
         <v>913</v>
       </c>
       <c r="C11" t="s">
-        <v>1038</v>
+        <v>996</v>
       </c>
       <c r="D11" t="s">
-        <v>1067</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+        <v>1025</v>
+      </c>
+      <c r="E11">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>1150</v>
+        <v>1106</v>
       </c>
       <c r="B12" t="s">
         <v>914</v>
       </c>
       <c r="D12" t="s">
-        <v>1068</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+        <v>1026</v>
+      </c>
+      <c r="E12">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>1151</v>
+        <v>1107</v>
       </c>
       <c r="B13" t="s">
         <v>918</v>
       </c>
       <c r="C13" t="s">
-        <v>1039</v>
+        <v>997</v>
       </c>
       <c r="D13" t="s">
-        <v>1069</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+        <v>1027</v>
+      </c>
+      <c r="E13">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>1152</v>
+        <v>1108</v>
       </c>
       <c r="B14" t="s">
         <v>920</v>
       </c>
       <c r="C14" t="s">
-        <v>1040</v>
+        <v>998</v>
       </c>
       <c r="D14" t="s">
-        <v>1070</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+        <v>1028</v>
+      </c>
+      <c r="E14">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>1153</v>
+        <v>1109</v>
       </c>
       <c r="B15" t="s">
         <v>927</v>
       </c>
       <c r="D15" t="s">
-        <v>1071</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+        <v>1029</v>
+      </c>
+      <c r="E15">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>1154</v>
+        <v>1110</v>
       </c>
       <c r="B16" t="s">
         <v>928</v>
       </c>
       <c r="C16" t="s">
-        <v>1041</v>
+        <v>999</v>
       </c>
       <c r="D16" t="s">
-        <v>1072</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+        <v>1030</v>
+      </c>
+      <c r="E16">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>1155</v>
+        <v>1111</v>
       </c>
       <c r="B17" t="s">
         <v>929</v>
       </c>
       <c r="C17" t="s">
-        <v>1042</v>
+        <v>1000</v>
       </c>
       <c r="D17" t="s">
-        <v>1073</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+        <v>1031</v>
+      </c>
+      <c r="E17">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>1156</v>
+        <v>1112</v>
       </c>
       <c r="B18" t="s">
         <v>930</v>
       </c>
       <c r="C18" t="s">
-        <v>1043</v>
+        <v>1001</v>
       </c>
       <c r="D18" t="s">
-        <v>1074</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+        <v>1032</v>
+      </c>
+      <c r="E18">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>1157</v>
+        <v>1113</v>
       </c>
       <c r="B19" t="s">
         <v>931</v>
       </c>
       <c r="C19" t="s">
-        <v>1044</v>
+        <v>1002</v>
       </c>
       <c r="D19" t="s">
-        <v>1075</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+        <v>1033</v>
+      </c>
+      <c r="E19">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>1158</v>
+        <v>1114</v>
       </c>
       <c r="B20" t="s">
         <v>932</v>
       </c>
       <c r="C20" t="s">
-        <v>1045</v>
+        <v>1003</v>
       </c>
       <c r="D20" t="s">
-        <v>1076</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+        <v>1034</v>
+      </c>
+      <c r="E20">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>1159</v>
+        <v>1115</v>
       </c>
       <c r="B21" t="s">
         <v>933</v>
       </c>
       <c r="C21" t="s">
-        <v>1046</v>
+        <v>1004</v>
       </c>
       <c r="D21" t="s">
-        <v>1077</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+        <v>1035</v>
+      </c>
+      <c r="E21">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>1160</v>
+        <v>1116</v>
       </c>
       <c r="B22" t="s">
         <v>934</v>
       </c>
       <c r="C22" t="s">
-        <v>1047</v>
+        <v>1005</v>
       </c>
       <c r="D22" t="s">
-        <v>1078</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+        <v>1036</v>
+      </c>
+      <c r="E22">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>1161</v>
+        <v>1117</v>
       </c>
       <c r="B23" t="s">
         <v>935</v>
       </c>
       <c r="C23" t="s">
-        <v>1048</v>
+        <v>1006</v>
       </c>
       <c r="D23" t="s">
-        <v>1079</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+        <v>1037</v>
+      </c>
+      <c r="E23">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>1162</v>
+        <v>1118</v>
       </c>
       <c r="B24" t="s">
         <v>937</v>
       </c>
       <c r="C24" t="s">
-        <v>1049</v>
+        <v>1007</v>
       </c>
       <c r="D24" t="s">
-        <v>1080</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+        <v>1038</v>
+      </c>
+      <c r="E24">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>1163</v>
+        <v>1119</v>
       </c>
       <c r="B25" t="s">
         <v>942</v>
       </c>
       <c r="C25" t="s">
-        <v>1050</v>
+        <v>1008</v>
       </c>
       <c r="D25" t="s">
-        <v>1081</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+        <v>1039</v>
+      </c>
+      <c r="E25">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>1164</v>
+        <v>1120</v>
       </c>
       <c r="B26" t="s">
         <v>943</v>
       </c>
       <c r="C26" t="s">
-        <v>1051</v>
+        <v>1009</v>
       </c>
       <c r="D26" t="s">
-        <v>1082</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+        <v>1040</v>
+      </c>
+      <c r="E26">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>1165</v>
+        <v>1121</v>
       </c>
       <c r="B27" t="s">
         <v>953</v>
       </c>
       <c r="C27" t="s">
-        <v>1052</v>
+        <v>1010</v>
       </c>
       <c r="D27" t="s">
-        <v>1083</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+        <v>1041</v>
+      </c>
+      <c r="E27">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>1166</v>
+        <v>1122</v>
       </c>
       <c r="B28" t="s">
         <v>954</v>
       </c>
       <c r="C28" t="s">
-        <v>1053</v>
+        <v>1011</v>
       </c>
       <c r="D28" t="s">
-        <v>1084</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+        <v>1042</v>
+      </c>
+      <c r="E28">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>1167</v>
+        <v>1123</v>
       </c>
       <c r="B29" t="s">
         <v>955</v>
       </c>
       <c r="C29" t="s">
-        <v>1054</v>
+        <v>1012</v>
       </c>
       <c r="D29" t="s">
-        <v>1085</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+        <v>1043</v>
+      </c>
+      <c r="E29">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>1168</v>
+        <v>1124</v>
       </c>
       <c r="B30" t="s">
         <v>956</v>
       </c>
       <c r="C30" t="s">
-        <v>1055</v>
+        <v>1013</v>
       </c>
       <c r="D30" t="s">
-        <v>1086</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+        <v>1044</v>
+      </c>
+      <c r="E30">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>1169</v>
+        <v>1125</v>
       </c>
       <c r="B31" t="s">
         <v>958</v>
       </c>
       <c r="C31" t="s">
-        <v>1056</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+        <v>1014</v>
+      </c>
+      <c r="E31">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>1170</v>
+        <v>1126</v>
       </c>
       <c r="B32" t="s">
         <v>960</v>
       </c>
       <c r="C32" t="s">
-        <v>1057</v>
+        <v>1015</v>
       </c>
       <c r="D32" t="s">
-        <v>1087</v>
+        <v>1045</v>
+      </c>
+      <c r="E32">
+        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -4496,8 +4476,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:E68"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+    <sheetView tabSelected="1" topLeftCell="B59" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4510,16 +4490,16 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>1135</v>
+        <v>1093</v>
       </c>
       <c r="B1" t="s">
-        <v>1137</v>
+        <v>1095</v>
       </c>
       <c r="C1" t="s">
         <v>37</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>1136</v>
+        <v>1094</v>
       </c>
       <c r="E1" t="s">
         <v>101</v>
@@ -4527,10 +4507,10 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>1088</v>
+        <v>1046</v>
       </c>
       <c r="B2" t="s">
-        <v>1088</v>
+        <v>1046</v>
       </c>
       <c r="C2" t="s">
         <v>103</v>
@@ -4544,10 +4524,10 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>1089</v>
+        <v>1047</v>
       </c>
       <c r="B3" t="s">
-        <v>1089</v>
+        <v>1047</v>
       </c>
       <c r="C3" t="s">
         <v>106</v>
@@ -4561,10 +4541,10 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>1090</v>
+        <v>1048</v>
       </c>
       <c r="B4" t="s">
-        <v>1090</v>
+        <v>1048</v>
       </c>
       <c r="C4" t="s">
         <v>109</v>
@@ -4578,10 +4558,10 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>1059</v>
+        <v>1017</v>
       </c>
       <c r="B5" t="s">
-        <v>1059</v>
+        <v>1017</v>
       </c>
       <c r="C5" t="s">
         <v>112</v>
@@ -4595,10 +4575,10 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>1060</v>
+        <v>1018</v>
       </c>
       <c r="B6" t="s">
-        <v>1060</v>
+        <v>1018</v>
       </c>
       <c r="C6" t="s">
         <v>115</v>
@@ -4612,10 +4592,10 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>1091</v>
+        <v>1049</v>
       </c>
       <c r="B7" t="s">
-        <v>1091</v>
+        <v>1049</v>
       </c>
       <c r="C7" t="s">
         <v>118</v>
@@ -4629,10 +4609,10 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>1061</v>
+        <v>1019</v>
       </c>
       <c r="B8" t="s">
-        <v>1061</v>
+        <v>1019</v>
       </c>
       <c r="C8" t="s">
         <v>121</v>
@@ -4646,10 +4626,10 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>1044</v>
+        <v>1002</v>
       </c>
       <c r="B9" t="s">
-        <v>1044</v>
+        <v>1002</v>
       </c>
       <c r="C9" t="s">
         <v>124</v>
@@ -4663,10 +4643,10 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>1092</v>
+        <v>1050</v>
       </c>
       <c r="B10" t="s">
-        <v>1092</v>
+        <v>1050</v>
       </c>
       <c r="C10" t="s">
         <v>127</v>
@@ -4680,10 +4660,10 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>1093</v>
+        <v>1051</v>
       </c>
       <c r="B11" t="s">
-        <v>1093</v>
+        <v>1051</v>
       </c>
       <c r="C11" t="s">
         <v>130</v>
@@ -4697,10 +4677,10 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>1094</v>
+        <v>1052</v>
       </c>
       <c r="B12" t="s">
-        <v>1094</v>
+        <v>1052</v>
       </c>
       <c r="C12" t="s">
         <v>133</v>
@@ -4714,10 +4694,10 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>1095</v>
+        <v>1053</v>
       </c>
       <c r="B13" t="s">
-        <v>1095</v>
+        <v>1053</v>
       </c>
       <c r="C13" t="s">
         <v>136</v>
@@ -4731,10 +4711,10 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>1096</v>
+        <v>1054</v>
       </c>
       <c r="B14" t="s">
-        <v>1096</v>
+        <v>1054</v>
       </c>
       <c r="C14" t="s">
         <v>139</v>
@@ -4748,10 +4728,10 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>1097</v>
+        <v>1055</v>
       </c>
       <c r="B15" t="s">
-        <v>1097</v>
+        <v>1055</v>
       </c>
       <c r="C15" t="s">
         <v>142</v>
@@ -4765,10 +4745,10 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>1098</v>
+        <v>1056</v>
       </c>
       <c r="B16" t="s">
-        <v>1098</v>
+        <v>1056</v>
       </c>
       <c r="C16" t="s">
         <v>145</v>
@@ -4782,10 +4762,10 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>1099</v>
+        <v>1057</v>
       </c>
       <c r="B17" t="s">
-        <v>1099</v>
+        <v>1057</v>
       </c>
       <c r="C17" t="s">
         <v>148</v>
@@ -4799,10 +4779,10 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>1100</v>
+        <v>1058</v>
       </c>
       <c r="B18" t="s">
-        <v>1100</v>
+        <v>1058</v>
       </c>
       <c r="C18" t="s">
         <v>151</v>
@@ -4816,10 +4796,10 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>1101</v>
+        <v>1059</v>
       </c>
       <c r="B19" t="s">
-        <v>1101</v>
+        <v>1059</v>
       </c>
       <c r="C19" t="s">
         <v>154</v>
@@ -4833,10 +4813,10 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>1102</v>
+        <v>1060</v>
       </c>
       <c r="B20" t="s">
-        <v>1102</v>
+        <v>1060</v>
       </c>
       <c r="C20" t="s">
         <v>157</v>
@@ -4850,10 +4830,10 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>1103</v>
+        <v>1061</v>
       </c>
       <c r="B21" t="s">
-        <v>1103</v>
+        <v>1061</v>
       </c>
       <c r="C21" t="s">
         <v>160</v>
@@ -4867,10 +4847,10 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>1104</v>
+        <v>1062</v>
       </c>
       <c r="B22" t="s">
-        <v>1104</v>
+        <v>1062</v>
       </c>
       <c r="C22" t="s">
         <v>163</v>
@@ -4884,10 +4864,10 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>1105</v>
+        <v>1063</v>
       </c>
       <c r="B23" t="s">
-        <v>1105</v>
+        <v>1063</v>
       </c>
       <c r="C23" t="s">
         <v>166</v>
@@ -4901,10 +4881,10 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>1106</v>
+        <v>1064</v>
       </c>
       <c r="B24" t="s">
-        <v>1106</v>
+        <v>1064</v>
       </c>
       <c r="C24" t="s">
         <v>169</v>
@@ -4918,10 +4898,10 @@
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>1070</v>
+        <v>1028</v>
       </c>
       <c r="B25" t="s">
-        <v>1070</v>
+        <v>1028</v>
       </c>
       <c r="C25" t="s">
         <v>172</v>
@@ -4935,10 +4915,10 @@
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>1107</v>
+        <v>1065</v>
       </c>
       <c r="B26" t="s">
-        <v>1107</v>
+        <v>1065</v>
       </c>
       <c r="C26" t="s">
         <v>175</v>
@@ -4952,10 +4932,10 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>1108</v>
+        <v>1066</v>
       </c>
       <c r="B27" t="s">
-        <v>1108</v>
+        <v>1066</v>
       </c>
       <c r="C27" t="s">
         <v>178</v>
@@ -4969,10 +4949,10 @@
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>1109</v>
+        <v>1067</v>
       </c>
       <c r="B28" t="s">
-        <v>1109</v>
+        <v>1067</v>
       </c>
       <c r="C28" t="s">
         <v>181</v>
@@ -4986,10 +4966,10 @@
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>1110</v>
+        <v>1068</v>
       </c>
       <c r="B29" t="s">
-        <v>1110</v>
+        <v>1068</v>
       </c>
       <c r="C29" t="s">
         <v>184</v>
@@ -5003,10 +4983,10 @@
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>1111</v>
+        <v>1069</v>
       </c>
       <c r="B30" t="s">
-        <v>1111</v>
+        <v>1069</v>
       </c>
       <c r="C30" t="s">
         <v>187</v>
@@ -5020,10 +5000,10 @@
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>1112</v>
+        <v>1070</v>
       </c>
       <c r="B31" t="s">
-        <v>1112</v>
+        <v>1070</v>
       </c>
       <c r="C31" t="s">
         <v>190</v>
@@ -5037,10 +5017,10 @@
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>1113</v>
+        <v>1071</v>
       </c>
       <c r="B32" t="s">
-        <v>1113</v>
+        <v>1071</v>
       </c>
       <c r="C32" t="s">
         <v>193</v>
@@ -5054,10 +5034,10 @@
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>1114</v>
+        <v>1072</v>
       </c>
       <c r="B33" t="s">
-        <v>1114</v>
+        <v>1072</v>
       </c>
       <c r="C33" t="s">
         <v>196</v>
@@ -5071,10 +5051,10 @@
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>1115</v>
+        <v>1073</v>
       </c>
       <c r="B34" t="s">
-        <v>1115</v>
+        <v>1073</v>
       </c>
       <c r="C34" t="s">
         <v>199</v>
@@ -5088,10 +5068,10 @@
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>1074</v>
+        <v>1032</v>
       </c>
       <c r="B35" t="s">
-        <v>1074</v>
+        <v>1032</v>
       </c>
       <c r="C35" t="s">
         <v>202</v>
@@ -5105,10 +5085,10 @@
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>1116</v>
+        <v>1074</v>
       </c>
       <c r="B36" t="s">
-        <v>1116</v>
+        <v>1074</v>
       </c>
       <c r="C36" t="s">
         <v>205</v>
@@ -5122,10 +5102,10 @@
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>1117</v>
+        <v>1075</v>
       </c>
       <c r="B37" t="s">
-        <v>1117</v>
+        <v>1075</v>
       </c>
       <c r="C37" t="s">
         <v>208</v>
@@ -5139,10 +5119,10 @@
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>1118</v>
+        <v>1076</v>
       </c>
       <c r="B38" t="s">
-        <v>1118</v>
+        <v>1076</v>
       </c>
       <c r="C38" t="s">
         <v>211</v>
@@ -5156,10 +5136,10 @@
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>1119</v>
+        <v>1077</v>
       </c>
       <c r="B39" t="s">
-        <v>1119</v>
+        <v>1077</v>
       </c>
       <c r="C39" t="s">
         <v>214</v>
@@ -5173,10 +5153,10 @@
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>1079</v>
+        <v>1037</v>
       </c>
       <c r="B40" t="s">
-        <v>1079</v>
+        <v>1037</v>
       </c>
       <c r="C40" t="s">
         <v>217</v>
@@ -5190,10 +5170,10 @@
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>1120</v>
+        <v>1078</v>
       </c>
       <c r="B41" t="s">
-        <v>1120</v>
+        <v>1078</v>
       </c>
       <c r="C41" t="s">
         <v>220</v>
@@ -5207,10 +5187,10 @@
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>1080</v>
+        <v>1038</v>
       </c>
       <c r="B42" t="s">
-        <v>1080</v>
+        <v>1038</v>
       </c>
       <c r="C42" t="s">
         <v>223</v>
@@ -5224,10 +5204,10 @@
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>1121</v>
+        <v>1079</v>
       </c>
       <c r="B43" t="s">
-        <v>1121</v>
+        <v>1079</v>
       </c>
       <c r="C43" t="s">
         <v>226</v>
@@ -5241,10 +5221,10 @@
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>1122</v>
+        <v>1080</v>
       </c>
       <c r="B44" t="s">
-        <v>1122</v>
+        <v>1080</v>
       </c>
       <c r="C44" t="s">
         <v>229</v>
@@ -5258,10 +5238,10 @@
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>1049</v>
+        <v>1007</v>
       </c>
       <c r="B45" t="s">
-        <v>1049</v>
+        <v>1007</v>
       </c>
       <c r="C45" t="s">
         <v>232</v>
@@ -5275,10 +5255,10 @@
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>1123</v>
+        <v>1081</v>
       </c>
       <c r="B46" t="s">
-        <v>1123</v>
+        <v>1081</v>
       </c>
       <c r="C46" t="s">
         <v>235</v>
@@ -5292,10 +5272,10 @@
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>1081</v>
+        <v>1039</v>
       </c>
       <c r="B47" t="s">
-        <v>1081</v>
+        <v>1039</v>
       </c>
       <c r="C47" t="s">
         <v>238</v>
@@ -5309,10 +5289,10 @@
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>1082</v>
+        <v>1040</v>
       </c>
       <c r="B48" t="s">
-        <v>1082</v>
+        <v>1040</v>
       </c>
       <c r="C48" t="s">
         <v>241</v>
@@ -5326,10 +5306,10 @@
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>1124</v>
+        <v>1082</v>
       </c>
       <c r="B49" t="s">
-        <v>1124</v>
+        <v>1082</v>
       </c>
       <c r="C49" t="s">
         <v>244</v>
@@ -5343,10 +5323,10 @@
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>1125</v>
+        <v>1083</v>
       </c>
       <c r="B50" t="s">
-        <v>1125</v>
+        <v>1083</v>
       </c>
       <c r="C50" t="s">
         <v>247</v>
@@ -5360,10 +5340,10 @@
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>1126</v>
+        <v>1084</v>
       </c>
       <c r="B51" t="s">
-        <v>1126</v>
+        <v>1084</v>
       </c>
       <c r="C51" t="s">
         <v>250</v>
@@ -5377,10 +5357,10 @@
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>1127</v>
+        <v>1085</v>
       </c>
       <c r="B52" t="s">
-        <v>1127</v>
+        <v>1085</v>
       </c>
       <c r="C52" t="s">
         <v>253</v>
@@ -5394,10 +5374,10 @@
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>1128</v>
+        <v>1086</v>
       </c>
       <c r="B53" t="s">
-        <v>1128</v>
+        <v>1086</v>
       </c>
       <c r="C53" t="s">
         <v>256</v>
@@ -5411,10 +5391,10 @@
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>1129</v>
+        <v>1087</v>
       </c>
       <c r="B54" t="s">
-        <v>1129</v>
+        <v>1087</v>
       </c>
       <c r="C54" t="s">
         <v>259</v>
@@ -5428,10 +5408,10 @@
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>1130</v>
+        <v>1088</v>
       </c>
       <c r="B55" t="s">
-        <v>1130</v>
+        <v>1088</v>
       </c>
       <c r="C55" t="s">
         <v>262</v>
@@ -5445,10 +5425,10 @@
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>1038</v>
+        <v>996</v>
       </c>
       <c r="B56" t="s">
-        <v>1038</v>
+        <v>996</v>
       </c>
       <c r="C56" t="s">
         <v>265</v>
@@ -5462,10 +5442,10 @@
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>1050</v>
+        <v>1008</v>
       </c>
       <c r="B57" t="s">
-        <v>1050</v>
+        <v>1008</v>
       </c>
       <c r="C57" t="s">
         <v>268</v>
@@ -5479,10 +5459,10 @@
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>1083</v>
+        <v>1041</v>
       </c>
       <c r="B58" t="s">
-        <v>1083</v>
+        <v>1041</v>
       </c>
       <c r="C58" t="s">
         <v>271</v>
@@ -5496,10 +5476,10 @@
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>1084</v>
+        <v>1042</v>
       </c>
       <c r="B59" t="s">
-        <v>1084</v>
+        <v>1042</v>
       </c>
       <c r="C59" t="s">
         <v>274</v>
@@ -5513,10 +5493,10 @@
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>1085</v>
+        <v>1043</v>
       </c>
       <c r="B60" t="s">
-        <v>1085</v>
+        <v>1043</v>
       </c>
       <c r="C60" t="s">
         <v>277</v>
@@ -5530,7 +5510,7 @@
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B61" t="s">
-        <v>1086</v>
+        <v>1044</v>
       </c>
       <c r="C61" t="s">
         <v>280</v>
@@ -5544,7 +5524,7 @@
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B62" t="s">
-        <v>1131</v>
+        <v>1089</v>
       </c>
       <c r="C62" t="s">
         <v>283</v>
@@ -5558,7 +5538,7 @@
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B63" t="s">
-        <v>1132</v>
+        <v>1090</v>
       </c>
       <c r="C63" t="s">
         <v>286</v>
@@ -5572,7 +5552,7 @@
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B64" t="s">
-        <v>1133</v>
+        <v>1091</v>
       </c>
       <c r="C64" t="s">
         <v>289</v>
@@ -5586,7 +5566,7 @@
     </row>
     <row r="65" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B65" t="s">
-        <v>1087</v>
+        <v>1045</v>
       </c>
       <c r="C65" t="s">
         <v>292</v>
@@ -5600,7 +5580,7 @@
     </row>
     <row r="66" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B66" t="s">
-        <v>1134</v>
+        <v>1092</v>
       </c>
       <c r="C66" t="s">
         <v>295</v>
@@ -5638,8 +5618,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C34BF907-426F-4FB9-9871-D5C6D8B21B3A}">
   <dimension ref="A1:G32"/>
   <sheetViews>
-    <sheetView zoomScale="121" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1:F1048576"/>
+    <sheetView topLeftCell="A19" zoomScale="121" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5659,22 +5639,22 @@
         <v>752</v>
       </c>
       <c r="B1" t="s">
+        <v>1130</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>964</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>1006</v>
-      </c>
       <c r="D1" s="1" t="s">
-        <v>1005</v>
+        <v>1131</v>
       </c>
       <c r="E1" t="s">
-        <v>963</v>
+        <v>1128</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>1007</v>
+        <v>965</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>1027</v>
+        <v>985</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -5688,13 +5668,13 @@
         <v>0</v>
       </c>
       <c r="E2" t="s">
-        <v>1003</v>
+        <v>1016</v>
       </c>
       <c r="F2" s="1">
         <v>25</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>1009</v>
+        <v>967</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -5702,22 +5682,22 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>965</v>
+        <v>989</v>
       </c>
       <c r="C3" s="1">
         <v>15</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>1008</v>
+        <v>966</v>
       </c>
       <c r="E3" t="s">
-        <v>111</v>
+        <v>1017</v>
       </c>
       <c r="F3" s="1">
         <v>2</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>1017</v>
+        <v>975</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -5725,22 +5705,22 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>966</v>
+        <v>990</v>
       </c>
       <c r="C4" s="1">
         <v>25</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>1009</v>
+        <v>967</v>
       </c>
       <c r="E4" t="s">
-        <v>114</v>
+        <v>1018</v>
       </c>
       <c r="F4" s="1">
         <v>3</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>1020</v>
+        <v>978</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -5748,22 +5728,22 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>967</v>
+        <v>991</v>
       </c>
       <c r="C5" s="1">
         <v>27</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>1010</v>
+        <v>968</v>
       </c>
       <c r="E5" t="s">
-        <v>120</v>
+        <v>1019</v>
       </c>
       <c r="F5" s="1">
         <v>3</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>1020</v>
+        <v>978</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -5771,22 +5751,22 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>968</v>
+        <v>992</v>
       </c>
       <c r="C6" s="1">
         <v>23</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>1011</v>
+        <v>969</v>
       </c>
       <c r="E6" t="s">
-        <v>1002</v>
+        <v>1020</v>
       </c>
       <c r="F6" s="1">
         <v>9</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>1018</v>
+        <v>976</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -5794,22 +5774,22 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>969</v>
+        <v>993</v>
       </c>
       <c r="C7" s="1">
         <v>13</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>1012</v>
+        <v>970</v>
       </c>
       <c r="E7" t="s">
-        <v>1001</v>
+        <v>1021</v>
       </c>
       <c r="F7" s="1">
         <v>11</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>1026</v>
+        <v>984</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -5823,7 +5803,7 @@
         <v>0</v>
       </c>
       <c r="E8" t="s">
-        <v>1000</v>
+        <v>1022</v>
       </c>
       <c r="F8" s="1">
         <v>12</v>
@@ -5837,7 +5817,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>970</v>
+        <v>994</v>
       </c>
       <c r="C9" s="1">
         <v>16</v>
@@ -5846,13 +5826,13 @@
         <v>20</v>
       </c>
       <c r="E9" t="s">
-        <v>999</v>
+        <v>1023</v>
       </c>
       <c r="F9" s="1">
         <v>5</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>1025</v>
+        <v>983</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -5860,22 +5840,22 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>971</v>
+        <v>995</v>
       </c>
       <c r="C10" s="1">
         <v>22</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>1013</v>
+        <v>971</v>
       </c>
       <c r="E10" t="s">
-        <v>998</v>
+        <v>1024</v>
       </c>
       <c r="F10" s="1">
         <v>14</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>1019</v>
+        <v>977</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
@@ -5883,7 +5863,7 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>264</v>
+        <v>996</v>
       </c>
       <c r="C11" s="1">
         <v>4</v>
@@ -5892,7 +5872,7 @@
         <v>5</v>
       </c>
       <c r="E11" t="s">
-        <v>997</v>
+        <v>1025</v>
       </c>
       <c r="F11" s="1">
         <v>8</v>
@@ -5912,13 +5892,13 @@
         <v>0</v>
       </c>
       <c r="E12" t="s">
-        <v>996</v>
+        <v>1026</v>
       </c>
       <c r="F12" s="1">
         <v>10</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>1023</v>
+        <v>981</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
@@ -5926,22 +5906,22 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>972</v>
+        <v>997</v>
       </c>
       <c r="C13" s="1">
         <v>21</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>1014</v>
+        <v>972</v>
       </c>
       <c r="E13" t="s">
-        <v>995</v>
+        <v>1027</v>
       </c>
       <c r="F13" s="1">
         <v>11</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>1026</v>
+        <v>984</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
@@ -5949,22 +5929,22 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>973</v>
+        <v>998</v>
       </c>
       <c r="C14" s="1">
         <v>31</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>1015</v>
+        <v>973</v>
       </c>
       <c r="E14" t="s">
-        <v>171</v>
+        <v>1028</v>
       </c>
       <c r="F14" s="1">
         <v>3</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>1020</v>
+        <v>978</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
@@ -5978,13 +5958,13 @@
         <v>0</v>
       </c>
       <c r="E15" t="s">
-        <v>994</v>
+        <v>1029</v>
       </c>
       <c r="F15" s="1">
         <v>10</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>1023</v>
+        <v>981</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
@@ -5992,7 +5972,7 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>974</v>
+        <v>999</v>
       </c>
       <c r="C16" s="1">
         <v>0</v>
@@ -6001,7 +5981,7 @@
         <v>0</v>
       </c>
       <c r="E16" t="s">
-        <v>993</v>
+        <v>1030</v>
       </c>
       <c r="F16" s="1">
         <v>0</v>
@@ -6015,7 +5995,7 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>975</v>
+        <v>1000</v>
       </c>
       <c r="C17" s="1">
         <v>24</v>
@@ -6024,13 +6004,13 @@
         <v>30</v>
       </c>
       <c r="E17" t="s">
-        <v>992</v>
+        <v>1031</v>
       </c>
       <c r="F17" s="1">
         <v>17</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>1021</v>
+        <v>979</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
@@ -6038,22 +6018,22 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>976</v>
+        <v>1001</v>
       </c>
       <c r="C18" s="1">
         <v>18</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>1016</v>
+        <v>974</v>
       </c>
       <c r="E18" t="s">
-        <v>201</v>
+        <v>1032</v>
       </c>
       <c r="F18" s="1">
         <v>3</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>1020</v>
+        <v>978</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
@@ -6061,22 +6041,22 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>123</v>
+        <v>1002</v>
       </c>
       <c r="C19" s="1">
         <v>2</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>1017</v>
+        <v>975</v>
       </c>
       <c r="E19" t="s">
-        <v>991</v>
+        <v>1033</v>
       </c>
       <c r="F19" s="1">
         <v>11</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>1026</v>
+        <v>984</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
@@ -6084,22 +6064,22 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>977</v>
+        <v>1003</v>
       </c>
       <c r="C20" s="1">
         <v>21</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>1014</v>
+        <v>972</v>
       </c>
       <c r="E20" t="s">
-        <v>990</v>
+        <v>1034</v>
       </c>
       <c r="F20" s="1">
         <v>19</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>1022</v>
+        <v>980</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
@@ -6107,7 +6087,7 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>978</v>
+        <v>1004</v>
       </c>
       <c r="C21" s="1">
         <v>20</v>
@@ -6116,13 +6096,13 @@
         <v>25</v>
       </c>
       <c r="E21" t="s">
-        <v>989</v>
+        <v>1035</v>
       </c>
       <c r="F21" s="1">
         <v>23</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>1011</v>
+        <v>969</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
@@ -6130,16 +6110,16 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>979</v>
+        <v>1005</v>
       </c>
       <c r="C22" s="1">
         <v>9</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>1018</v>
+        <v>976</v>
       </c>
       <c r="E22" t="s">
-        <v>988</v>
+        <v>1036</v>
       </c>
       <c r="F22" s="1">
         <v>28</v>
@@ -6153,22 +6133,22 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>980</v>
+        <v>1006</v>
       </c>
       <c r="C23" s="1">
         <v>14</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>1019</v>
+        <v>977</v>
       </c>
       <c r="E23" t="s">
-        <v>216</v>
+        <v>1037</v>
       </c>
       <c r="F23" s="1">
         <v>3</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>1020</v>
+        <v>978</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
@@ -6176,22 +6156,22 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>231</v>
+        <v>1007</v>
       </c>
       <c r="C24" s="1">
         <v>3</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>1020</v>
+        <v>978</v>
       </c>
       <c r="E24" t="s">
-        <v>222</v>
+        <v>1038</v>
       </c>
       <c r="F24" s="1">
         <v>1</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>1024</v>
+        <v>982</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
@@ -6199,22 +6179,22 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>267</v>
+        <v>1008</v>
       </c>
       <c r="C25" s="1">
         <v>2</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>1017</v>
+        <v>975</v>
       </c>
       <c r="E25" t="s">
-        <v>237</v>
+        <v>1039</v>
       </c>
       <c r="F25" s="1">
         <v>1</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>1024</v>
+        <v>982</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
@@ -6222,22 +6202,22 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>981</v>
+        <v>1009</v>
       </c>
       <c r="C26" s="1">
         <v>17</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>1021</v>
+        <v>979</v>
       </c>
       <c r="E26" t="s">
-        <v>240</v>
+        <v>1040</v>
       </c>
       <c r="F26" s="1">
         <v>3</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>1020</v>
+        <v>978</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
@@ -6245,22 +6225,22 @@
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>982</v>
+        <v>1010</v>
       </c>
       <c r="C27" s="1">
         <v>3</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>1020</v>
+        <v>978</v>
       </c>
       <c r="E27" t="s">
-        <v>270</v>
+        <v>1041</v>
       </c>
       <c r="F27" s="1">
         <v>3</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>1020</v>
+        <v>978</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
@@ -6268,22 +6248,22 @@
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>983</v>
+        <v>1011</v>
       </c>
       <c r="C28" s="1">
         <v>19</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>1022</v>
+        <v>980</v>
       </c>
       <c r="E28" t="s">
-        <v>273</v>
+        <v>1042</v>
       </c>
       <c r="F28" s="1">
         <v>5</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>1025</v>
+        <v>983</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
@@ -6291,7 +6271,7 @@
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>984</v>
+        <v>1012</v>
       </c>
       <c r="C29" s="1">
         <v>8</v>
@@ -6300,13 +6280,13 @@
         <v>10</v>
       </c>
       <c r="E29" t="s">
-        <v>276</v>
+        <v>1043</v>
       </c>
       <c r="F29" s="1">
         <v>1</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>1024</v>
+        <v>982</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
@@ -6314,22 +6294,22 @@
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>985</v>
+        <v>1013</v>
       </c>
       <c r="C30" s="1">
         <v>10</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>1023</v>
+        <v>981</v>
       </c>
       <c r="E30" t="s">
-        <v>279</v>
+        <v>1044</v>
       </c>
       <c r="F30" s="1">
         <v>2</v>
       </c>
       <c r="G30" s="1" t="s">
-        <v>1017</v>
+        <v>975</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
@@ -6337,13 +6317,13 @@
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>986</v>
+        <v>1014</v>
       </c>
       <c r="C31" s="1">
         <v>14</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>1019</v>
+        <v>977</v>
       </c>
       <c r="F31" s="1">
         <v>0</v>
@@ -6357,22 +6337,22 @@
         <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>987</v>
+        <v>1015</v>
       </c>
       <c r="C32" s="1">
         <v>19</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>1022</v>
+        <v>980</v>
       </c>
       <c r="E32" t="s">
-        <v>291</v>
+        <v>1045</v>
       </c>
       <c r="F32" s="1">
         <v>2</v>
       </c>
       <c r="G32" s="1" t="s">
-        <v>1017</v>
+        <v>975</v>
       </c>
     </row>
   </sheetData>
@@ -6392,10 +6372,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>1029</v>
+        <v>987</v>
       </c>
       <c r="B1" t="s">
-        <v>1028</v>
+        <v>986</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -13509,7 +13489,7 @@
         <v>100</v>
       </c>
       <c r="B1" t="s">
-        <v>1004</v>
+        <v>963</v>
       </c>
       <c r="C1" t="s">
         <v>775</v>

</xml_diff>